<commit_message>
Updated website and codebook
</commit_message>
<xml_diff>
--- a/i_codebooks/D4_persontime_Cube_ImmDis.xlsx
+++ b/i_codebooks/D4_persontime_Cube_ImmDis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18_Objective_2\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\Pipeline_template_CoMaSy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB53F74-61EB-45E5-B732-2AAF7494156D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Parameters" sheetId="5" r:id="rId3"/>
     <sheet name="Example" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -288,7 +289,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,7 +480,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -756,20 +757,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.88671875" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -777,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -785,7 +786,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -793,7 +794,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -801,13 +802,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -815,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -823,17 +824,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -848,7 +849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -858,23 +859,23 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.77734375" style="9" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="9"/>
+    <col min="9" max="9" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" style="9" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -910,7 +911,7 @@
       </c>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>76</v>
       </c>
@@ -932,7 +933,7 @@
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>72</v>
       </c>
@@ -954,7 +955,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>73</v>
       </c>
@@ -976,7 +977,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
     </row>
-    <row r="5" spans="1:12" ht="69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>50</v>
       </c>
@@ -996,7 +997,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>56</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>67</v>
       </c>
@@ -1023,7 +1024,7 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>57</v>
       </c>
@@ -1044,23 +1045,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1164,7 +1165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1178,7 +1179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1192,7 +1193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1206,7 +1207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1226,23 +1227,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A27" sqref="A27:A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>76</v>
       </c>
@@ -1267,7 +1268,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>1</v>
       </c>
@@ -1428,7 +1429,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>1</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>1</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>1</v>
       </c>
@@ -1499,7 +1500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>1</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>1</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>1</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>1</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>1</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>1</v>
       </c>
@@ -1649,7 +1650,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>76</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
         <v>1</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="22">
         <v>1</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>1</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <v>1</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>1</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>1</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <v>1</v>
       </c>
@@ -1785,7 +1786,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>1</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <v>1</v>
       </c>

</xml_diff>